<commit_message>
Add item panel and icons of item and frame
</commit_message>
<xml_diff>
--- a/DataSource/excel/npc.xlsx
+++ b/DataSource/excel/npc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="960" windowWidth="24640" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="npc.csv" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,53 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Yujie Liu</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yujie Liu:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="2"/>
+            <charset val="134"/>
+          </rPr>
+          <t>男，
+0：女</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
   <si>
     <t>id</t>
   </si>
@@ -115,13 +160,16 @@
   </si>
   <si>
     <t>portraitPosY</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +206,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -526,20 +594,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -550,55 +618,58 @@
         <v>25</v>
       </c>
       <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -609,25 +680,25 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>7</v>
+      <c r="F2" t="s">
+        <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
         <v>2</v>
@@ -636,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="N2" t="s">
         <v>7</v>
@@ -654,10 +725,13 @@
         <v>7</v>
       </c>
       <c r="S2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3">
         <v>1</v>
       </c>
@@ -667,56 +741,59 @@
       <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
         <v>20</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>100</v>
       </c>
-      <c r="J3" t="s">
-        <v>1</v>
-      </c>
       <c r="K3" t="s">
         <v>1</v>
       </c>
       <c r="L3" t="s">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3">
         <v>95</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>75</v>
       </c>
-      <c r="O3">
-        <v>80</v>
-      </c>
       <c r="P3">
         <v>80</v>
       </c>
       <c r="Q3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="R3">
         <v>50</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3">
+        <v>50</v>
+      </c>
+      <c r="T3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4">
         <v>2</v>
       </c>
@@ -726,35 +803,35 @@
       <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4">
-        <v>2</v>
+      <c r="D4" s="1">
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2">
         <v>31</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>10</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>100</v>
       </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
       <c r="K4" t="s">
         <v>1</v>
       </c>
       <c r="L4" t="s">
         <v>1</v>
       </c>
-      <c r="M4">
-        <v>80</v>
+      <c r="M4" t="s">
+        <v>1</v>
       </c>
       <c r="N4">
         <v>80</v>
@@ -766,16 +843,19 @@
         <v>80</v>
       </c>
       <c r="Q4">
+        <v>80</v>
+      </c>
+      <c r="R4">
         <v>90</v>
       </c>
-      <c r="R4">
-        <v>80</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="S4">
+        <v>80</v>
+      </c>
+      <c r="T4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5">
         <v>3</v>
       </c>
@@ -785,35 +865,35 @@
       <c r="C5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>20</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
       <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>100</v>
       </c>
-      <c r="J5" t="s">
-        <v>1</v>
-      </c>
       <c r="K5" t="s">
         <v>1</v>
       </c>
       <c r="L5" t="s">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>80</v>
+      <c r="M5" t="s">
+        <v>1</v>
       </c>
       <c r="N5">
         <v>80</v>
@@ -830,13 +910,17 @@
       <c r="R5">
         <v>80</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5">
+        <v>80</v>
+      </c>
+      <c r="T5" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
small change of role panel
</commit_message>
<xml_diff>
--- a/DataSource/excel/npc.xlsx
+++ b/DataSource/excel/npc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="960" windowWidth="24640" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="npc.csv" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>charm</t>
   </si>
   <si>
-    <t>lucky</t>
-  </si>
-  <si>
     <t>skillList</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>弗里奥</t>
+  </si>
+  <si>
+    <t>luck</t>
   </si>
 </sst>
 </file>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -631,28 +631,28 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -676,13 +676,13 @@
         <v>14</v>
       </c>
       <c r="R1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
         <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -755,7 +755,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -806,7 +806,7 @@
         <v>50</v>
       </c>
       <c r="T3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -814,10 +814,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
@@ -868,7 +868,7 @@
         <v>80</v>
       </c>
       <c r="T4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -876,10 +876,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -930,7 +930,7 @@
         <v>80</v>
       </c>
       <c r="T5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -938,10 +938,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -992,7 +992,7 @@
         <v>80</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:20">
@@ -1000,10 +1000,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -1054,7 +1054,7 @@
         <v>80</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add select cannon. But I still need to add the outline and do the city-cannon-money things.
</commit_message>
<xml_diff>
--- a/DataSource/excel/npc.xlsx
+++ b/DataSource/excel/npc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="25360" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="npc.csv" sheetId="1" r:id="rId1"/>
@@ -651,7 +651,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Add ship info scene, small changes of shipunit panel
</commit_message>
<xml_diff>
--- a/DataSource/excel/npc.xlsx
+++ b/DataSource/excel/npc.xlsx
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>